<commit_message>
added mar 3, 2020 data
</commit_message>
<xml_diff>
--- a/Water_Chemistry/Data/Titrator/TrisCalibration.xlsx
+++ b/Water_Chemistry/Data/Titrator/TrisCalibration.xlsx
@@ -8,30 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/Water_Chemistry/Data/Titrator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED912F0E-CB59-734D-9BB4-2183A85B3914}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5A57AB-00EE-FF49-BBD0-01F5CD249370}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="1100" windowWidth="23960" windowHeight="11180" firstSheet="6" activeTab="16" xr2:uid="{CFC1D0D6-766B-0649-B317-8AE9A7B8F3ED}"/>
+    <workbookView xWindow="1500" yWindow="1460" windowWidth="23960" windowHeight="11180" firstSheet="7" activeTab="18" xr2:uid="{CFC1D0D6-766B-0649-B317-8AE9A7B8F3ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nov7" sheetId="1" r:id="rId1"/>
-    <sheet name="Nov12" sheetId="2" r:id="rId2"/>
-    <sheet name="Nov16" sheetId="3" r:id="rId3"/>
-    <sheet name="Nov19" sheetId="4" r:id="rId4"/>
-    <sheet name="Nov28" sheetId="7" r:id="rId5"/>
-    <sheet name="Dec05" sheetId="5" r:id="rId6"/>
-    <sheet name="Dec12" sheetId="6" r:id="rId7"/>
-    <sheet name="Dec19" sheetId="8" r:id="rId8"/>
-    <sheet name="Jan2" sheetId="12" r:id="rId9"/>
-    <sheet name="Jan3" sheetId="9" r:id="rId10"/>
-    <sheet name="Jan14" sheetId="11" r:id="rId11"/>
-    <sheet name="May29" sheetId="13" r:id="rId12"/>
-    <sheet name="Sept6" sheetId="14" r:id="rId13"/>
-    <sheet name="Sept13" sheetId="15" r:id="rId14"/>
-    <sheet name="Sept19" sheetId="16" r:id="rId15"/>
-    <sheet name="Sept27" sheetId="17" r:id="rId16"/>
-    <sheet name="19Dec2019" sheetId="19" r:id="rId17"/>
-    <sheet name="Oct11" sheetId="18" r:id="rId18"/>
-    <sheet name="Sheet2" sheetId="20" r:id="rId19"/>
+    <sheet name="20181107" sheetId="1" r:id="rId1"/>
+    <sheet name="20181112" sheetId="2" r:id="rId2"/>
+    <sheet name="20181116" sheetId="3" r:id="rId3"/>
+    <sheet name="20181119" sheetId="4" r:id="rId4"/>
+    <sheet name="20181128" sheetId="7" r:id="rId5"/>
+    <sheet name="20181205" sheetId="5" r:id="rId6"/>
+    <sheet name="20181212" sheetId="6" r:id="rId7"/>
+    <sheet name="20181219" sheetId="8" r:id="rId8"/>
+    <sheet name="20190102" sheetId="12" r:id="rId9"/>
+    <sheet name="20190103" sheetId="9" r:id="rId10"/>
+    <sheet name="20190114" sheetId="11" r:id="rId11"/>
+    <sheet name="20190529" sheetId="13" r:id="rId12"/>
+    <sheet name="20190906" sheetId="14" r:id="rId13"/>
+    <sheet name="20190913" sheetId="15" r:id="rId14"/>
+    <sheet name="20190919" sheetId="16" r:id="rId15"/>
+    <sheet name="20190927" sheetId="17" r:id="rId16"/>
+    <sheet name="20191219" sheetId="19" r:id="rId17"/>
+    <sheet name="20191011" sheetId="18" r:id="rId18"/>
+    <sheet name="20200303" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="6">
   <si>
     <t>pH</t>
   </si>
@@ -85,12 +85,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,11 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,7 +189,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Nov7'!$D$1</c:f>
+              <c:f>'20181107'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -265,7 +272,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov7'!$D$2:$D$13</c:f>
+              <c:f>'20181107'!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -310,7 +317,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov7'!$C$2:$C$13</c:f>
+              <c:f>'20181107'!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -706,7 +713,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jan2'!$D$2:$D$8</c:f>
+              <c:f>'20190102'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -736,7 +743,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jan2'!$C$2:$C$8</c:f>
+              <c:f>'20190102'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1079,7 +1086,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jan3'!$D$2:$D$8</c:f>
+              <c:f>'20190103'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1109,7 +1116,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jan3'!$C$2:$C$8</c:f>
+              <c:f>'20190103'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1458,7 +1465,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jan14'!$C$4:$C$17</c:f>
+              <c:f>'20190114'!$C$4:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1503,7 +1510,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jan14'!$D$4:$D$17</c:f>
+              <c:f>'20190114'!$D$4:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1867,7 +1874,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jan14'!$C$2:$C$15</c:f>
+              <c:f>'20190114'!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1918,7 +1925,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jan14'!$D$2:$D$15</c:f>
+              <c:f>'20190114'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2288,7 +2295,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sept6!$C$2:$C$18</c:f>
+              <c:f>'20190906'!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2348,7 +2355,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sept6!$D$2:$D$18</c:f>
+              <c:f>'20190906'!$D$2:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2727,7 +2734,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sept13!$C$2:$C$18</c:f>
+              <c:f>'20190913'!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2787,7 +2794,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sept13!$D$2:$D$18</c:f>
+              <c:f>'20190913'!$D$2:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3166,7 +3173,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sept19!$C$4:$C$19</c:f>
+              <c:f>'20190919'!$C$4:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3223,7 +3230,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sept19!$D$4:$D$19</c:f>
+              <c:f>'20190919'!$D$4:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3599,7 +3606,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sept27!$C$2:$C$15</c:f>
+              <c:f>'20190927'!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="14"/>
@@ -3650,7 +3657,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sept27!$D$2:$D$15</c:f>
+              <c:f>'20190927'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -4033,7 +4040,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'19Dec2019'!$C$10:$C$20</c:f>
+              <c:f>'20191219'!$C$10:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4075,7 +4082,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'19Dec2019'!$D$10:$D$20</c:f>
+              <c:f>'20191219'!$D$10:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4309,6 +4316,427 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.17976946631671042"/>
+                  <c:y val="0.12279199475065616"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'20200303'!$D$4:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>8.8800000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'20200303'!$C$4:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-84.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-84.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-84.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-84.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-83.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-83.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-82.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-82.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-81.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-81.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-81</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-80.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A00-C243-9E7B-DE8C22AA84D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1214357007"/>
+        <c:axId val="1264420175"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1214357007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1264420175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1264420175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1214357007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -4364,7 +4792,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Nov7'!$D$1</c:f>
+              <c:f>'20181107'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4447,7 +4875,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov7'!$D$6:$D$13</c:f>
+              <c:f>'20181107'!$D$6:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4480,7 +4908,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov7'!$C$6:$C$13</c:f>
+              <c:f>'20181107'!$C$6:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4858,7 +5286,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov12'!$D$2:$D$17</c:f>
+              <c:f>'20181112'!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4915,7 +5343,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov12'!$C$2:$C$17</c:f>
+              <c:f>'20181112'!$C$2:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -5241,7 +5669,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov16'!$D$2:$D$13</c:f>
+              <c:f>'20181116'!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5286,7 +5714,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov16'!$C$2:$C$13</c:f>
+              <c:f>'20181116'!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5407,7 +5835,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov16'!$D$5:$D$13</c:f>
+              <c:f>'20181116'!$D$5:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -5443,7 +5871,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov16'!$C$5:$C$13</c:f>
+              <c:f>'20181116'!$C$5:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -5792,7 +6220,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov19'!$E$2:$E$20</c:f>
+              <c:f>'20181119'!$E$2:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -5801,7 +6229,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov19'!$D$2:$D$20</c:f>
+              <c:f>'20181119'!$D$2:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -6099,7 +6527,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Nov28'!$B$6</c:f>
+              <c:f>'20181128'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6176,7 +6604,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Nov28'!$D$2:$D$15</c:f>
+              <c:f>'20181128'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -6227,7 +6655,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Nov28'!$C$2:$C$15</c:f>
+              <c:f>'20181128'!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -6591,7 +7019,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dec05'!$D$6:$D$20</c:f>
+              <c:f>'20181205'!$D$6:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -6645,7 +7073,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dec05'!$C$6:$C$20</c:f>
+              <c:f>'20181205'!$C$6:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -7012,7 +7440,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dec05'!$D$2:$D$20</c:f>
+              <c:f>'20181205'!$D$2:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7078,7 +7506,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dec05'!$C$2:$C$20</c:f>
+              <c:f>'20181205'!$C$2:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7457,7 +7885,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dec19'!$D$2:$D$24</c:f>
+              <c:f>'20181219'!$D$2:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -7535,7 +7963,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dec19'!$C$2:$C$24</c:f>
+              <c:f>'20181219'!$C$2:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -8205,6 +8633,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -13170,6 +13638,522 @@
 </file>
 
 <file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18220,6 +19204,47 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B460C77A-8841-5741-8956-66417123171A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -19363,7 +20388,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20838,8 +21863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4E2077-BC31-2C4F-BEED-753B2030501C}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21210,13 +22235,229 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B64B1874-9BBA-7748-A96F-467284B3F89A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20200303</v>
+      </c>
+      <c r="C2">
+        <v>-85.1</v>
+      </c>
+      <c r="D2">
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20200303</v>
+      </c>
+      <c r="C3">
+        <v>-84.8</v>
+      </c>
+      <c r="D3">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20200303</v>
+      </c>
+      <c r="C4" s="4">
+        <v>-84.7</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20200303</v>
+      </c>
+      <c r="C5" s="4">
+        <v>-84.2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.4600000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20200303</v>
+      </c>
+      <c r="C6" s="4">
+        <v>-84.1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20200303</v>
+      </c>
+      <c r="C7" s="4">
+        <v>-84.1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20200303</v>
+      </c>
+      <c r="C8" s="4">
+        <v>-83.9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10.119999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20200303</v>
+      </c>
+      <c r="C9" s="4">
+        <v>-83.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>10.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>20200303</v>
+      </c>
+      <c r="C10" s="4">
+        <v>-82.8</v>
+      </c>
+      <c r="D10" s="4">
+        <v>11.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>20200303</v>
+      </c>
+      <c r="C11" s="4">
+        <v>-82.4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>11.61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20200303</v>
+      </c>
+      <c r="C12" s="4">
+        <v>-81.900000000000006</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20200303</v>
+      </c>
+      <c r="C13" s="4">
+        <v>-81.599999999999994</v>
+      </c>
+      <c r="D13" s="4">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>20200303</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-81</v>
+      </c>
+      <c r="D14" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>20200303</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-80.400000000000006</v>
+      </c>
+      <c r="D15" s="4">
+        <v>13.52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20200303</v>
+      </c>
+      <c r="C16" s="4">
+        <v>-80</v>
+      </c>
+      <c r="D16" s="4">
+        <v>13.92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>20200303</v>
+      </c>
+      <c r="C17" s="4">
+        <v>-79</v>
+      </c>
+      <c r="D17" s="4">
+        <v>14.83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>20200303</v>
+      </c>
+      <c r="C18">
+        <v>-78.2</v>
+      </c>
+      <c r="D18">
+        <v>15.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>20200303</v>
+      </c>
+      <c r="C19">
+        <v>-78.099999999999994</v>
+      </c>
+      <c r="D19">
+        <v>15.51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>